<commit_message>
add ant config to execute excel cases
</commit_message>
<xml_diff>
--- a/BMW_IAT/resources/reward.xlsx
+++ b/BMW_IAT/resources/reward.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>CaseID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>2015/03/02 17:51:13</t>
+  </si>
+  <si>
+    <t>2015/03/04 15:27:38</t>
+  </si>
+  <si>
+    <t>2015/03/04 15:28:34</t>
   </si>
 </sst>
 </file>
@@ -1171,7 +1177,7 @@
         <v>25</v>
       </c>
       <c r="C2" s="45" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="46"/>
       <c r="E2" s="49"/>

</xml_diff>